<commit_message>
MSHub new retention index.
</commit_message>
<xml_diff>
--- a/MSHub_RT_IDs.xlsx
+++ b/MSHub_RT_IDs.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MSHub" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="MSHub_2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t xml:space="preserve">Identification level</t>
   </si>
@@ -52,7 +53,160 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">NIST#: 162948</t>
+    <t xml:space="preserve">Butanoic acid / Ethylacetic acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butanoic acid, ethyl ester / Ethyl butyrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pentanedinitrile, 2-methyl- / Methylglutaronitrile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3-Diazabicyclo[3.2.2]nonan-4-one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,3,4,4-Tetramethyl-cyclopentanone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethanedial, dioxime /  Glyoxime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexane, 3,3-dimethyl- / 3,3-Dimethylhexane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Hexene, 3,5,5-trimethyl- / 3,5,5-Trimethyl-hex-2-ene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2-Heptanediol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pentanedioic acid, monomethyl ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4-Nonanedione, 5-ethyl-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexanoic acid, 2,2-dimethyl- / </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Hydroxymethyl-2-methylcyclopentanol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Undecene, 4-methyl- / 4-Methyl-1-undecene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutaric acid, 3-methylbut-2-yl 3-hexyl ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclohexane, 2,4-diisopropyl-1,1-dimethyl-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclohexyl methylphosphonate / Cyclohexyl hydrogen methylphosphonate  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,5,7-Trimethyl-1,2(4H)-diazepine / 3,5,7-Trimethyl-4H-1,2-diazepine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tetrahydrofuran-2-one, 5-[1-hydroxyhexyl]-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-[(Z)-1-Butenyl]-1,4-cycloheptadiene / Ectocarpene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxiranecarboxaldehyde, 3-methyl-3-(4-methyl-3-pentenyl)- / 3-Methyl-3-(4-methyl-3-pentenyl)-2-oxiranecarbaldehyde  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,7-Nonadien-4-ol, 4,8-dimethyl- / 4,8-Dimethyl-1,7-nonadien-4-ol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimethyl-1,8-naphthalenedioxysilane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9-Decyn-1-ol / 9-Decynyl alcohol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-Tetradecen-3-yne, (Z)- / (5Z)-5-Tetradecen-3-yne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Acetyl-3-methylbenzo[b]thiophene / 1-(3-Methyl-1-benzothien-2-yl)ethanone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-(5-(1-hydroxyethyl)-5-methyl-tetrahydrofuran-2-yl)propan-1-ol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-(5-(1-hydroxyethyl)-5-methyl-tetrahydrofuran-2-yl)propan-1-ol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodeca-1,6-dien-12-ol, 6,10-dimethyl- / (6Z)-3,7-Dimethyl-6,11-dodecadien-1-ol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclohexanecarboxylic acid, 4-(1,5-dimethyl-3-oxohexyl)-, methyl ester, cis- / Methyl 4-(1,5-dimethyl-3-oxohexyl)cyclohexanecarboxylate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-Undecyn-1-ol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimethylmalonic acid, monochloride, 3-phenylpropyl ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambrial / γ-Bicyclohomofarnesal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycloheptanone, 3-butyl- / Butylcycloheptanone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butyl citrate / Citric acid, tributyl ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Methyl-3-(3-methyl-but-2-enyl)-2-(4-methyl-pent-3-enyl)-oxetane / 2-Methyl-3-(3-methyl-2-butenyl)-2-(4-methyl-3-pentenyl)oxetane  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-2 Tetraol / T-2 toxin tetraol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pentadecanal- / 1-Pentadecanal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,4,8a(6H)-Anthracenetriol, 5,7,8,9,10,10a-hexahydro-5,5-dimethyl- / 5,5-Dimethyl-5,7,8,9,10,10a-hexahydro-1,4,8a(6H)-anthracenetriol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexadecanoic acid, 2-hydroxy-1-(hydroxymethyl)ethyl ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heptasiloxane, hexadecamethyl- / Hexadecamethylheptasiloxane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2,3-Diphenylcyclopropyl)methyl phenyl sulfoxide, trans-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heptacosane / n-Heptacosane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbonic acid, eicosyl vinyl ester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undecane, 4,6-dimethyl- / 4,6-Dimethylundecane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farnesol (E), methyl ether </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methyl tetratriacontyl ether </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docosane, 1-iodo- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,9,13,17-Tetramethyl 4,8,12,16-octadecatetraenoic acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,8,12-Tetradecatrienal, 5,9,13-trimethyl- / (4E,8E)-5,9,13-Trimethyl-4,8,12-tetradecatrienal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,6,10,15,19,23-Pentamethyl-2,6,18,22-tetracosatetraen-10,15-diol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eicosane, 2-methyl-</t>
   </si>
 </sst>
 </file>
@@ -63,7 +217,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -85,6 +239,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,7 +290,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -147,6 +308,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,7 +334,7 @@
   </sheetPr>
   <dimension ref="A1:J309"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -210,7 +375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="n">
         <v>4</v>
       </c>
@@ -219,19 +384,10 @@
         <v>3.46</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="n">
-        <v>837</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <f aca="false">ABS(E2-F2)</f>
-        <v>837</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>0.773</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
@@ -2689,6 +2845,918 @@
         <v>54.91</v>
       </c>
     </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J309"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="12.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>8.81</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>11.45</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>229</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>12.92</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>13.64</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>249</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>14.08</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>14.34</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>277</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>15.34</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>309</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>16.6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>17.18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>319</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>17.35</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>373</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>19.6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>21.44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>22.84</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="n">
+        <v>508</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>24.38</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="n">
+        <v>518</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>24.56</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="n">
+        <v>570</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>26.46</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="n">
+        <v>585</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>27.21</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="n">
+        <v>637</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="4" t="n">
+        <v>29.53</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="n">
+        <v>656</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>30.18</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="n">
+        <v>661</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="4" t="n">
+        <v>30.58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="n">
+        <v>693</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>31.76</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="n">
+        <v>703</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="4" t="n">
+        <v>32.28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <v>714</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>32.78</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="n">
+        <v>742</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="4" t="n">
+        <v>33.83</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <v>747</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>33.95</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="n">
+        <v>752</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="4" t="n">
+        <v>34.27</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="n">
+        <v>776</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>35.34</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="n">
+        <v>833</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="4" t="n">
+        <v>37.39</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="n">
+        <v>856</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>37.97</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>879</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="4" t="n">
+        <v>39.18</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>927</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>40.96</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="n">
+        <v>971</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="4" t="n">
+        <v>42.1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="n">
+        <v>992</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>43.04</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="n">
+        <v>996</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="4" t="n">
+        <v>43.25</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="n">
+        <v>1002</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>43.58</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="n">
+        <v>1005</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="4" t="n">
+        <v>43.99</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="n">
+        <v>1026</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>45.14</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="n">
+        <v>1039</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="4" t="n">
+        <v>45.47</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="n">
+        <v>1050</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>45.85</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="n">
+        <v>1077</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="4" t="n">
+        <v>46.84</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="n">
+        <v>1101</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>47.65</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="n">
+        <v>1171</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="4" t="n">
+        <v>51.16</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="n">
+        <v>1180</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>51.62</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="n">
+        <v>1187</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="4" t="n">
+        <v>51.99</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="n">
+        <v>1240</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="4" t="n">
+        <v>54.78</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>